<commit_message>
Næsten i mål med logikken
</commit_message>
<xml_diff>
--- a/statChoser/data.xlsx
+++ b/statChoser/data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="137">
   <si>
     <t>id</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Q9</t>
   </si>
   <si>
-    <t>Underlying distribution normal or can central-limit theorem be assumed to hold?</t>
-  </si>
-  <si>
     <t>Q4</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t>Normal-theory methods pages 245-246</t>
   </si>
   <si>
-    <t>two-sample problem</t>
-  </si>
-  <si>
     <t>Q38</t>
   </si>
   <si>
@@ -153,9 +147,6 @@
     <t>Q15</t>
   </si>
   <si>
-    <t>Are samples independent?</t>
-  </si>
-  <si>
     <t>Q14</t>
   </si>
   <si>
@@ -264,9 +255,6 @@
     <t>Nonparametric ANOVA - Kruskal-wallis test. P 556-557</t>
   </si>
   <si>
-    <t>Other covariates to be controlled for?</t>
-  </si>
-  <si>
     <t>one-way anova p 516-538</t>
   </si>
   <si>
@@ -415,6 +403,33 @@
   </si>
   <si>
     <t>question</t>
+  </si>
+  <si>
+    <t>Other covariates to be controlled for? (Q27)</t>
+  </si>
+  <si>
+    <t>Other covariates to be controlled for? (Q28)</t>
+  </si>
+  <si>
+    <t>Other covariates to be controlled for? (Q25)</t>
+  </si>
+  <si>
+    <t>Are samples independent? (Q13)</t>
+  </si>
+  <si>
+    <t>Are samples independent? (Q17)</t>
+  </si>
+  <si>
+    <t>Underlying distribution normal or can central-limit theorem be assumed to hold? (Q3)</t>
+  </si>
+  <si>
+    <t>Underlying distribution normal or can central-limit theorem be assumed to hold? (Q10)</t>
+  </si>
+  <si>
+    <t>two-sample problem (Q9)</t>
+  </si>
+  <si>
+    <t>two-sample problem (Q32)</t>
   </si>
 </sst>
 </file>
@@ -734,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,7 +767,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -825,13 +840,13 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
         <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -839,153 +854,153 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>133</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
         <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
         <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
         <v>22</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
         <v>24</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>25</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E14" t="s">
         <v>26</v>
-      </c>
-      <c r="E14" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
         <v>24</v>
       </c>
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
       <c r="C15" t="s">
         <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
         <v>29</v>
-      </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -993,13 +1008,13 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
         <v>32</v>
-      </c>
-      <c r="C18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1007,237 +1022,237 @@
         <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>135</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>134</v>
       </c>
       <c r="C20" t="s">
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" t="s">
+        <v>134</v>
+      </c>
+      <c r="C21" t="s">
         <v>34</v>
       </c>
-      <c r="B21" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" t="s">
-        <v>36</v>
-      </c>
       <c r="D21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
         <v>38</v>
-      </c>
-      <c r="C22" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
         <v>41</v>
-      </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" t="s">
+        <v>131</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" t="s">
         <v>42</v>
-      </c>
-      <c r="B26" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>131</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
       </c>
       <c r="E27" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C28" t="s">
         <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
       </c>
       <c r="E29" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
       </c>
       <c r="E30" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C31" t="s">
         <v>5</v>
       </c>
       <c r="D31" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>44</v>
+        <v>132</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
       </c>
       <c r="E32" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>44</v>
+        <v>132</v>
       </c>
       <c r="C33" t="s">
         <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B34" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C34" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E34" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" t="s">
         <v>52</v>
-      </c>
-      <c r="B35" t="s">
-        <v>53</v>
-      </c>
-      <c r="C35" t="s">
-        <v>5</v>
-      </c>
-      <c r="E35" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1245,13 +1260,13 @@
         <v>8</v>
       </c>
       <c r="B36" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C36" t="s">
         <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1259,671 +1274,671 @@
         <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C37" t="s">
         <v>6</v>
       </c>
       <c r="D37" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
         <v>57</v>
-      </c>
-      <c r="B38" t="s">
-        <v>59</v>
-      </c>
-      <c r="C38" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B39" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C39" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D39" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B40" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C40" t="s">
         <v>5</v>
       </c>
       <c r="E40" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
       </c>
       <c r="D41" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>64</v>
+      </c>
+      <c r="B42" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" t="s">
         <v>67</v>
-      </c>
-      <c r="B42" t="s">
-        <v>68</v>
-      </c>
-      <c r="C42" t="s">
-        <v>5</v>
-      </c>
-      <c r="E42" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B43" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C43" t="s">
         <v>6</v>
       </c>
       <c r="E43" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B44" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C44" t="s">
         <v>5</v>
       </c>
       <c r="D44" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B45" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C45" t="s">
         <v>6</v>
       </c>
       <c r="D45" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B46" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C46">
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B47" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C47">
         <v>2</v>
       </c>
       <c r="D47" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B48" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C48">
         <v>3</v>
       </c>
       <c r="D48" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>72</v>
+      </c>
+      <c r="B49" t="s">
         <v>75</v>
       </c>
-      <c r="B49" t="s">
-        <v>78</v>
-      </c>
       <c r="C49" t="s">
         <v>5</v>
       </c>
       <c r="D49" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>72</v>
+      </c>
+      <c r="B50" t="s">
         <v>75</v>
       </c>
-      <c r="B50" t="s">
-        <v>78</v>
-      </c>
       <c r="C50" t="s">
         <v>6</v>
       </c>
       <c r="E50" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>76</v>
+      </c>
+      <c r="B51" t="s">
+        <v>130</v>
+      </c>
+      <c r="C51" t="s">
+        <v>5</v>
+      </c>
+      <c r="E51" t="s">
         <v>79</v>
-      </c>
-      <c r="B51" t="s">
-        <v>81</v>
-      </c>
-      <c r="C51" t="s">
-        <v>5</v>
-      </c>
-      <c r="E51" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B52" t="s">
-        <v>81</v>
+        <v>130</v>
       </c>
       <c r="C52" t="s">
         <v>6</v>
       </c>
       <c r="E52" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B53" t="s">
-        <v>81</v>
+        <v>128</v>
       </c>
       <c r="C53" t="s">
         <v>5</v>
       </c>
       <c r="E53" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B54" t="s">
+        <v>128</v>
+      </c>
+      <c r="C54" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" t="s">
         <v>81</v>
-      </c>
-      <c r="C54" t="s">
-        <v>6</v>
-      </c>
-      <c r="E54" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B55" t="s">
-        <v>81</v>
+        <v>129</v>
       </c>
       <c r="C55" t="s">
         <v>5</v>
       </c>
       <c r="E55" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B56" t="s">
-        <v>81</v>
+        <v>129</v>
       </c>
       <c r="C56" t="s">
         <v>6</v>
       </c>
       <c r="E56" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C57" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D57" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B58" t="s">
+        <v>84</v>
+      </c>
+      <c r="C58" t="s">
+        <v>86</v>
+      </c>
+      <c r="E58" t="s">
         <v>88</v>
-      </c>
-      <c r="C58" t="s">
-        <v>90</v>
-      </c>
-      <c r="E58" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B59" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C59" t="s">
         <v>5</v>
       </c>
       <c r="D59" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B60" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C60" t="s">
         <v>6</v>
       </c>
       <c r="E60" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B61" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C61" t="s">
         <v>6</v>
       </c>
       <c r="D61" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B62" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C62" t="s">
         <v>5</v>
       </c>
       <c r="E62" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B63" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C63" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E63" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>92</v>
+      </c>
+      <c r="B64" t="s">
+        <v>93</v>
+      </c>
+      <c r="C64" t="s">
         <v>96</v>
       </c>
-      <c r="B64" t="s">
+      <c r="E64" t="s">
         <v>97</v>
-      </c>
-      <c r="C64" t="s">
-        <v>100</v>
-      </c>
-      <c r="E64" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B65" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C65" t="s">
         <v>5</v>
       </c>
       <c r="E65" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B66" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C66" t="s">
         <v>6</v>
       </c>
       <c r="D66" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>99</v>
+      </c>
+      <c r="B67" t="s">
+        <v>101</v>
+      </c>
+      <c r="C67" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67" t="s">
         <v>103</v>
-      </c>
-      <c r="B67" t="s">
-        <v>105</v>
-      </c>
-      <c r="C67" t="s">
-        <v>5</v>
-      </c>
-      <c r="D67" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B68" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C68" t="s">
         <v>6</v>
       </c>
       <c r="D68" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B69" t="s">
-        <v>32</v>
+        <v>136</v>
       </c>
       <c r="C69" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E69" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B70" t="s">
-        <v>32</v>
+        <v>136</v>
       </c>
       <c r="C70" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E70" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>102</v>
+      </c>
+      <c r="B71" t="s">
         <v>106</v>
       </c>
-      <c r="B71" t="s">
-        <v>110</v>
-      </c>
       <c r="C71" t="s">
         <v>5</v>
       </c>
       <c r="E71" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>102</v>
+      </c>
+      <c r="B72" t="s">
         <v>106</v>
       </c>
-      <c r="B72" t="s">
-        <v>110</v>
-      </c>
       <c r="C72" t="s">
         <v>6</v>
       </c>
       <c r="D72" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B73" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C73" t="s">
         <v>5</v>
       </c>
       <c r="E73" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B74" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C74" t="s">
         <v>6</v>
       </c>
       <c r="E74" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B75" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C75" t="s">
         <v>5</v>
       </c>
       <c r="E75" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B76" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C76" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D76" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B77" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C77" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D77" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B78" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C78" t="s">
         <v>6</v>
       </c>
       <c r="E78" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B79" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C79" t="s">
         <v>5</v>
       </c>
       <c r="E79" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B80" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C80" t="s">
         <v>6</v>
       </c>
       <c r="D80" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B81" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C81" t="s">
         <v>5</v>
       </c>
       <c r="E81" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>119</v>
+      </c>
+      <c r="B82" t="s">
+        <v>121</v>
+      </c>
+      <c r="C82" t="s">
+        <v>6</v>
+      </c>
+      <c r="E82" t="s">
         <v>123</v>
-      </c>
-      <c r="B82" t="s">
-        <v>125</v>
-      </c>
-      <c r="C82" t="s">
-        <v>6</v>
-      </c>
-      <c r="E82" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B83" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C83" t="s">
         <v>5</v>
       </c>
       <c r="E83" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B84" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C84" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E84" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nyt placeholder link - og et korrekt link
</commit_message>
<xml_diff>
--- a/statChoser/data.xlsx
+++ b/statChoser/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10632"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10635"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="175">
   <si>
     <t>id</t>
   </si>
@@ -447,9 +447,6 @@
     <t>Other covariates to be controlled for?</t>
   </si>
   <si>
-    <t>https://kubdatalab.github.io/R-toolbox/tidy-data.html</t>
-  </si>
-  <si>
     <t>one-sample z test pp 220-21 $\mu$</t>
   </si>
   <si>
@@ -541,6 +538,12 @@
   </si>
   <si>
     <t>Is the underlying distribution normal or can the central-limit theorem be assumed to hold? (Q10)</t>
+  </si>
+  <si>
+    <t>https://kubdatalab.github.io/R-toolbox/stat-tests-1.html#one-sample-z-test</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=_7zHp51j2WM</t>
   </si>
 </sst>
 </file>
@@ -872,27 +875,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.44140625" customWidth="1"/>
-    <col min="3" max="3" width="62.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" customWidth="1"/>
+    <col min="1" max="2" width="4.42578125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="62.7109375" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="22" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="42.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C1" t="s">
         <v>127</v>
@@ -907,7 +909,7 @@
         <v>132</v>
       </c>
       <c r="G1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H1" t="s">
         <v>128</v>
@@ -922,15 +924,15 @@
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -939,24 +941,24 @@
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D3" t="s">
         <v>25</v>
@@ -965,21 +967,21 @@
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
@@ -994,12 +996,12 @@
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D5" t="s">
         <v>25</v>
@@ -1014,12 +1016,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
@@ -1034,12 +1036,12 @@
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D7" t="s">
         <v>25</v>
@@ -1054,15 +1056,15 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
@@ -1071,24 +1073,24 @@
         <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I8" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D9" t="s">
         <v>25</v>
@@ -1097,10 +1099,10 @@
         <v>11</v>
       </c>
       <c r="G9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I9" t="s">
         <v>134</v>
@@ -1109,41 +1111,41 @@
         <v>11</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D10" t="s">
         <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I10" t="s">
         <v>135</v>
       </c>
       <c r="J10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D11" t="s">
         <v>25</v>
@@ -1152,7 +1154,7 @@
         <v>12</v>
       </c>
       <c r="H11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I11" t="s">
         <v>134</v>
@@ -1161,15 +1163,15 @@
         <v>12</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D12" t="s">
         <v>16</v>
@@ -1178,18 +1180,18 @@
         <v>13</v>
       </c>
       <c r="H12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I12" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D13" t="s">
         <v>25</v>
@@ -1198,18 +1200,18 @@
         <v>14</v>
       </c>
       <c r="H13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I13" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -1227,15 +1229,15 @@
         <v>17</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D15" t="s">
         <v>25</v>
@@ -1253,18 +1255,18 @@
         <v>18</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D16" t="s">
         <v>16</v>
@@ -1282,18 +1284,18 @@
         <v>21</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D17" t="s">
         <v>25</v>
@@ -1311,10 +1313,10 @@
         <v>20</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1334,7 +1336,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1354,12 +1356,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D20" t="s">
         <v>16</v>
@@ -1374,12 +1376,12 @@
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D21" t="s">
         <v>25</v>
@@ -1394,7 +1396,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1414,7 +1416,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1437,15 +1439,15 @@
         <v>28</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D24" t="s">
         <v>16</v>
@@ -1460,12 +1462,12 @@
         <v>135</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D25" t="s">
         <v>25</v>
@@ -1480,12 +1482,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D26" t="s">
         <v>16</v>
@@ -1500,12 +1502,12 @@
         <v>135</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>31</v>
       </c>
       <c r="C27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D27" t="s">
         <v>25</v>
@@ -1523,10 +1525,10 @@
         <v>50</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1546,7 +1548,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1569,10 +1571,10 @@
         <v>52</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1595,10 +1597,10 @@
         <v>37</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1618,12 +1620,12 @@
         <v>135</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
       <c r="C32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D32" t="s">
         <v>25</v>
@@ -1641,15 +1643,15 @@
         <v>39</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>29</v>
       </c>
       <c r="C33" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D33" t="s">
         <v>16</v>
@@ -1664,7 +1666,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -1687,10 +1689,10 @@
         <v>42</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -1713,10 +1715,10 @@
         <v>43</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -1736,7 +1738,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -1756,12 +1758,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>45</v>
       </c>
       <c r="C38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D38" t="s">
         <v>16</v>
@@ -1776,12 +1778,12 @@
         <v>135</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>45</v>
       </c>
       <c r="C39" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D39" t="s">
         <v>25</v>
@@ -1796,7 +1798,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>48</v>
       </c>
@@ -1819,10 +1821,10 @@
         <v>54</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>48</v>
       </c>
@@ -1842,7 +1844,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>55</v>
       </c>
@@ -1865,10 +1867,10 @@
         <v>58</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>55</v>
       </c>
@@ -1891,10 +1893,10 @@
         <v>57</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>49</v>
       </c>
@@ -1914,7 +1916,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -1934,15 +1936,15 @@
         <v>134</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>61</v>
       </c>
       <c r="B46" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C46" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -1951,7 +1953,7 @@
         <v>63</v>
       </c>
       <c r="G46" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H46" t="s">
         <v>62</v>
@@ -1960,15 +1962,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>61</v>
       </c>
       <c r="B47" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C47" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D47">
         <v>2</v>
@@ -1977,7 +1979,7 @@
         <v>64</v>
       </c>
       <c r="G47" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H47" t="s">
         <v>62</v>
@@ -1986,15 +1988,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>61</v>
       </c>
       <c r="B48" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C48" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D48">
         <v>3</v>
@@ -2003,7 +2005,7 @@
         <v>65</v>
       </c>
       <c r="G48" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H48" t="s">
         <v>62</v>
@@ -2012,7 +2014,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>63</v>
       </c>
@@ -2032,7 +2034,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>63</v>
       </c>
@@ -2055,10 +2057,10 @@
         <v>68</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>67</v>
       </c>
@@ -2081,10 +2083,10 @@
         <v>70</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>67</v>
       </c>
@@ -2107,10 +2109,10 @@
         <v>69</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>64</v>
       </c>
@@ -2133,10 +2135,10 @@
         <v>71</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>64</v>
       </c>
@@ -2159,10 +2161,10 @@
         <v>72</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>65</v>
       </c>
@@ -2185,10 +2187,10 @@
         <v>73</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>65</v>
       </c>
@@ -2211,10 +2213,10 @@
         <v>74</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>46</v>
       </c>
@@ -2234,7 +2236,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>46</v>
       </c>
@@ -2257,10 +2259,10 @@
         <v>79</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>78</v>
       </c>
@@ -2280,7 +2282,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>78</v>
       </c>
@@ -2303,10 +2305,10 @@
         <v>81</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -2326,7 +2328,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -2349,10 +2351,10 @@
         <v>57</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>83</v>
       </c>
@@ -2375,10 +2377,10 @@
         <v>86</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>83</v>
       </c>
@@ -2401,10 +2403,10 @@
         <v>88</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>38</v>
       </c>
@@ -2427,10 +2429,10 @@
         <v>91</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>38</v>
       </c>
@@ -2450,7 +2452,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>90</v>
       </c>
@@ -2470,7 +2472,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>90</v>
       </c>
@@ -2490,7 +2492,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>94</v>
       </c>
@@ -2513,10 +2515,10 @@
         <v>95</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>94</v>
       </c>
@@ -2539,18 +2541,18 @@
         <v>96</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>93</v>
       </c>
       <c r="B71" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C71" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D71" t="s">
         <v>16</v>
@@ -2568,18 +2570,18 @@
         <v>98</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>93</v>
       </c>
       <c r="B72" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C72" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D72" t="s">
         <v>25</v>
@@ -2594,15 +2596,15 @@
         <v>134</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>99</v>
       </c>
       <c r="B73" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C73" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D73" t="s">
         <v>16</v>
@@ -2620,18 +2622,18 @@
         <v>101</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>99</v>
       </c>
       <c r="B74" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C74" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D74" t="s">
         <v>25</v>
@@ -2649,10 +2651,10 @@
         <v>102</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>35</v>
       </c>
@@ -2675,10 +2677,10 @@
         <v>104</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>35</v>
       </c>
@@ -2698,7 +2700,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>105</v>
       </c>
@@ -2718,7 +2720,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>105</v>
       </c>
@@ -2741,10 +2743,10 @@
         <v>108</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>22</v>
       </c>
@@ -2767,10 +2769,10 @@
         <v>111</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>22</v>
       </c>
@@ -2790,7 +2792,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>110</v>
       </c>
@@ -2813,10 +2815,10 @@
         <v>113</v>
       </c>
       <c r="K81" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>110</v>
       </c>
@@ -2839,10 +2841,10 @@
         <v>114</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>107</v>
       </c>
@@ -2865,10 +2867,10 @@
         <v>116</v>
       </c>
       <c r="K83" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>107</v>
       </c>
@@ -2891,7 +2893,7 @@
         <v>117</v>
       </c>
       <c r="K84" s="1" t="s">
-        <v>142</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hm. Nok noget med nogen links.
</commit_message>
<xml_diff>
--- a/statChoser/data.xlsx
+++ b/statChoser/data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="178">
   <si>
     <t>id</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Inferences concerning means?</t>
   </si>
   <si>
-    <t>inferences concerning variances: Tow-sample F test to compare variances. (Caution: This test is very sensitive to nonnormality) p 284</t>
-  </si>
-  <si>
     <t>Q17</t>
   </si>
   <si>
@@ -544,6 +541,18 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=_7zHp51j2WM</t>
+  </si>
+  <si>
+    <t>https://kubdatalab.github.io/R-toolbox/stat-tests-1.html#one-sample-chi-square-test</t>
+  </si>
+  <si>
+    <t>https://kubdatalab.github.io/R-toolbox/stat-tests-1.html#one-sample-poisson-test</t>
+  </si>
+  <si>
+    <t>inferences concerning variances: Two-sample F test to compare variances. (Caution: This test is very sensitive to nonnormality) p 284</t>
+  </si>
+  <si>
+    <t>https://kubdatalab.github.io/R-toolbox/stat-tests-1.html#two-sample-f-test</t>
   </si>
 </sst>
 </file>
@@ -876,7 +885,7 @@
   <dimension ref="A1:K84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,34 +903,34 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
       </c>
       <c r="F1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J1" t="s">
+        <v>130</v>
+      </c>
+      <c r="K1" t="s">
         <v>132</v>
-      </c>
-      <c r="G1" t="s">
-        <v>152</v>
-      </c>
-      <c r="H1" t="s">
-        <v>128</v>
-      </c>
-      <c r="I1" t="s">
-        <v>129</v>
-      </c>
-      <c r="J1" t="s">
-        <v>131</v>
-      </c>
-      <c r="K1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -929,10 +938,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -941,13 +950,13 @@
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -955,10 +964,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D3" t="s">
         <v>25</v>
@@ -967,13 +976,13 @@
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -981,7 +990,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
@@ -993,7 +1002,7 @@
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1001,7 +1010,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D5" t="s">
         <v>25</v>
@@ -1013,7 +1022,7 @@
         <v>5</v>
       </c>
       <c r="I5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1021,7 +1030,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
@@ -1030,10 +1039,10 @@
         <v>8</v>
       </c>
       <c r="H6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1041,7 +1050,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D7" t="s">
         <v>25</v>
@@ -1050,10 +1059,10 @@
         <v>9</v>
       </c>
       <c r="H7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1061,10 +1070,10 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
@@ -1073,13 +1082,13 @@
         <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1087,10 +1096,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D9" t="s">
         <v>25</v>
@@ -1099,13 +1108,13 @@
         <v>11</v>
       </c>
       <c r="G9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J9" t="s">
         <v>11</v>
@@ -1119,25 +1128,25 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D10" t="s">
         <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1145,7 +1154,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D11" t="s">
         <v>25</v>
@@ -1154,10 +1163,10 @@
         <v>12</v>
       </c>
       <c r="H11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J11" t="s">
         <v>12</v>
@@ -1171,7 +1180,7 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D12" t="s">
         <v>16</v>
@@ -1180,10 +1189,10 @@
         <v>13</v>
       </c>
       <c r="H12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1191,7 +1200,7 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D13" t="s">
         <v>25</v>
@@ -1200,10 +1209,10 @@
         <v>14</v>
       </c>
       <c r="H13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1211,7 +1220,7 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -1223,13 +1232,13 @@
         <v>15</v>
       </c>
       <c r="I14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J14" t="s">
         <v>17</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1237,7 +1246,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D15" t="s">
         <v>25</v>
@@ -1249,13 +1258,13 @@
         <v>15</v>
       </c>
       <c r="I15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J15" t="s">
         <v>18</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1263,10 +1272,10 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D16" t="s">
         <v>16</v>
@@ -1278,13 +1287,13 @@
         <v>19</v>
       </c>
       <c r="I16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J16" t="s">
         <v>21</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1292,10 +1301,10 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D17" t="s">
         <v>25</v>
@@ -1307,13 +1316,13 @@
         <v>19</v>
       </c>
       <c r="I17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J17" t="s">
         <v>20</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1321,7 +1330,7 @@
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D18" t="s">
         <v>16</v>
@@ -1330,10 +1339,10 @@
         <v>23</v>
       </c>
       <c r="H18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1341,7 +1350,7 @@
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D19" t="s">
         <v>25</v>
@@ -1350,10 +1359,10 @@
         <v>22</v>
       </c>
       <c r="H19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1361,7 +1370,7 @@
         <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D20" t="s">
         <v>16</v>
@@ -1370,10 +1379,10 @@
         <v>24</v>
       </c>
       <c r="H20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1381,7 +1390,7 @@
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D21" t="s">
         <v>25</v>
@@ -1390,10 +1399,10 @@
         <v>26</v>
       </c>
       <c r="H21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1407,13 +1416,13 @@
         <v>16</v>
       </c>
       <c r="E22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H22" t="s">
         <v>27</v>
       </c>
       <c r="I22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1427,19 +1436,19 @@
         <v>25</v>
       </c>
       <c r="F23" t="s">
-        <v>28</v>
+        <v>176</v>
       </c>
       <c r="H23" t="s">
         <v>27</v>
       </c>
       <c r="I23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J23" t="s">
-        <v>28</v>
+        <v>176</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1447,19 +1456,19 @@
         <v>26</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D24" t="s">
         <v>16</v>
       </c>
       <c r="E24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1467,255 +1476,255 @@
         <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D25" t="s">
         <v>25</v>
       </c>
       <c r="E25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D26" t="s">
         <v>16</v>
       </c>
       <c r="E26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D27" t="s">
         <v>25</v>
       </c>
       <c r="F27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" t="s">
         <v>33</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" t="s">
         <v>34</v>
       </c>
-      <c r="D28" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" t="s">
-        <v>35</v>
-      </c>
       <c r="H28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" t="s">
         <v>33</v>
       </c>
-      <c r="C29" t="s">
-        <v>34</v>
-      </c>
       <c r="D29" t="s">
         <v>25</v>
       </c>
       <c r="F29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" t="s">
         <v>36</v>
       </c>
-      <c r="D30" t="s">
-        <v>25</v>
-      </c>
-      <c r="F30" t="s">
-        <v>37</v>
-      </c>
       <c r="H30" t="s">
+        <v>35</v>
+      </c>
+      <c r="I30" t="s">
+        <v>133</v>
+      </c>
+      <c r="J30" t="s">
         <v>36</v>
       </c>
-      <c r="I30" t="s">
-        <v>134</v>
-      </c>
-      <c r="J30" t="s">
-        <v>37</v>
-      </c>
       <c r="K30" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D31" t="s">
         <v>16</v>
       </c>
       <c r="E31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D32" t="s">
         <v>25</v>
       </c>
       <c r="F32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H32" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D33" t="s">
         <v>16</v>
       </c>
       <c r="E33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" t="s">
+        <v>138</v>
+      </c>
+      <c r="D34" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" t="s">
+        <v>41</v>
+      </c>
+      <c r="H34" t="s">
         <v>40</v>
       </c>
-      <c r="C34" t="s">
-        <v>139</v>
-      </c>
-      <c r="D34" t="s">
-        <v>25</v>
-      </c>
-      <c r="F34" t="s">
-        <v>42</v>
-      </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
+        <v>133</v>
+      </c>
+      <c r="J34" t="s">
         <v>41</v>
       </c>
-      <c r="I34" t="s">
-        <v>134</v>
-      </c>
-      <c r="J34" t="s">
-        <v>42</v>
-      </c>
       <c r="K34" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" t="s">
+        <v>138</v>
+      </c>
+      <c r="D35" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35" t="s">
+        <v>42</v>
+      </c>
+      <c r="H35" t="s">
         <v>40</v>
       </c>
-      <c r="C35" t="s">
-        <v>139</v>
-      </c>
-      <c r="D35" t="s">
-        <v>16</v>
-      </c>
-      <c r="F35" t="s">
-        <v>43</v>
-      </c>
-      <c r="H35" t="s">
-        <v>41</v>
-      </c>
       <c r="I35" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -1723,19 +1732,19 @@
         <v>4</v>
       </c>
       <c r="C36" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" t="s">
         <v>44</v>
       </c>
-      <c r="D36" t="s">
-        <v>16</v>
-      </c>
-      <c r="E36" t="s">
-        <v>45</v>
-      </c>
       <c r="H36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I36" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -1743,220 +1752,220 @@
         <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D37" t="s">
         <v>25</v>
       </c>
       <c r="E37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I37" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C38" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D38" t="s">
         <v>16</v>
       </c>
       <c r="E38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H38" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D39" t="s">
         <v>25</v>
       </c>
       <c r="E39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I39" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C40" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40" t="s">
+        <v>16</v>
+      </c>
+      <c r="F40" t="s">
         <v>53</v>
       </c>
-      <c r="D40" t="s">
-        <v>16</v>
-      </c>
-      <c r="F40" t="s">
-        <v>54</v>
-      </c>
       <c r="H40" t="s">
+        <v>52</v>
+      </c>
+      <c r="I40" t="s">
+        <v>134</v>
+      </c>
+      <c r="J40" t="s">
         <v>53</v>
       </c>
-      <c r="I40" t="s">
-        <v>135</v>
-      </c>
-      <c r="J40" t="s">
-        <v>54</v>
-      </c>
       <c r="K40" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D41" t="s">
         <v>25</v>
       </c>
       <c r="E41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" t="s">
         <v>55</v>
       </c>
-      <c r="C42" t="s">
-        <v>56</v>
-      </c>
       <c r="D42" t="s">
         <v>16</v>
       </c>
       <c r="F42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I42" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" t="s">
         <v>55</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F43" t="s">
         <v>56</v>
       </c>
-      <c r="D43" t="s">
-        <v>25</v>
-      </c>
-      <c r="F43" t="s">
-        <v>57</v>
-      </c>
       <c r="H43" t="s">
+        <v>55</v>
+      </c>
+      <c r="I43" t="s">
+        <v>133</v>
+      </c>
+      <c r="J43" t="s">
         <v>56</v>
       </c>
-      <c r="I43" t="s">
-        <v>134</v>
-      </c>
-      <c r="J43" t="s">
-        <v>57</v>
-      </c>
       <c r="K43" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D44" t="s">
         <v>16</v>
       </c>
       <c r="E44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I44" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C45" t="s">
+        <v>58</v>
+      </c>
+      <c r="D45" t="s">
+        <v>25</v>
+      </c>
+      <c r="E45" t="s">
         <v>59</v>
       </c>
-      <c r="D45" t="s">
-        <v>25</v>
-      </c>
-      <c r="E45" t="s">
-        <v>60</v>
-      </c>
       <c r="H45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I45" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B46" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C46" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D46">
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G46" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I46">
         <v>1</v>
@@ -1964,25 +1973,25 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B47" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D47">
         <v>2</v>
       </c>
       <c r="E47" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G47" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H47" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I47">
         <v>2</v>
@@ -1990,25 +1999,25 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B48" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C48" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D48">
         <v>3</v>
       </c>
       <c r="E48" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G48" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H48" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I48">
         <v>3</v>
@@ -2016,734 +2025,734 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C49" t="s">
+        <v>65</v>
+      </c>
+      <c r="D49" t="s">
+        <v>16</v>
+      </c>
+      <c r="E49" t="s">
         <v>66</v>
       </c>
-      <c r="D49" t="s">
-        <v>16</v>
-      </c>
-      <c r="E49" t="s">
-        <v>67</v>
-      </c>
       <c r="H49" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I49" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C50" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D50" t="s">
         <v>25</v>
       </c>
       <c r="F50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H50" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I50" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C51" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D51" t="s">
         <v>16</v>
       </c>
       <c r="F51" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H51" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I51" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J51" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C52" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D52" t="s">
         <v>25</v>
       </c>
       <c r="F52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H52" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I52" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C53" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D53" t="s">
         <v>16</v>
       </c>
       <c r="F53" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H53" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I53" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J53" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C54" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D54" t="s">
         <v>25</v>
       </c>
       <c r="F54" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H54" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I54" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J54" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C55" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D55" t="s">
         <v>16</v>
       </c>
       <c r="F55" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H55" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I55" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J55" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C56" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D56" t="s">
         <v>25</v>
       </c>
       <c r="F56" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H56" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I56" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J56" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C57" t="s">
+        <v>74</v>
+      </c>
+      <c r="D57" t="s">
         <v>75</v>
       </c>
-      <c r="D57" t="s">
-        <v>76</v>
-      </c>
       <c r="E57" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H57" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I57" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C58" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D58" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H58" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I58" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D59" t="s">
         <v>16</v>
       </c>
       <c r="E59" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I59" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C60" t="s">
+        <v>79</v>
+      </c>
+      <c r="D60" t="s">
+        <v>25</v>
+      </c>
+      <c r="F60" t="s">
         <v>80</v>
       </c>
-      <c r="D60" t="s">
-        <v>25</v>
-      </c>
-      <c r="F60" t="s">
-        <v>81</v>
-      </c>
       <c r="H60" t="s">
+        <v>79</v>
+      </c>
+      <c r="I60" t="s">
+        <v>133</v>
+      </c>
+      <c r="J60" t="s">
         <v>80</v>
       </c>
-      <c r="I60" t="s">
-        <v>134</v>
-      </c>
-      <c r="J60" t="s">
-        <v>81</v>
-      </c>
       <c r="K60" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C61" t="s">
+        <v>81</v>
+      </c>
+      <c r="D61" t="s">
+        <v>25</v>
+      </c>
+      <c r="E61" t="s">
         <v>82</v>
       </c>
-      <c r="D61" t="s">
-        <v>25</v>
-      </c>
-      <c r="E61" t="s">
-        <v>83</v>
-      </c>
       <c r="H61" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I61" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C62" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D62" t="s">
         <v>16</v>
       </c>
       <c r="F62" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H62" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I62" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J62" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>82</v>
+      </c>
+      <c r="C63" t="s">
         <v>83</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>84</v>
       </c>
-      <c r="D63" t="s">
+      <c r="F63" t="s">
         <v>85</v>
       </c>
-      <c r="F63" t="s">
-        <v>86</v>
-      </c>
       <c r="H63" t="s">
+        <v>83</v>
+      </c>
+      <c r="I63" t="s">
         <v>84</v>
       </c>
-      <c r="I63" t="s">
+      <c r="J63" t="s">
         <v>85</v>
       </c>
-      <c r="J63" t="s">
-        <v>86</v>
-      </c>
       <c r="K63" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>82</v>
+      </c>
+      <c r="C64" t="s">
         <v>83</v>
       </c>
-      <c r="C64" t="s">
-        <v>84</v>
-      </c>
       <c r="D64" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F64" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H64" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I64" t="s">
+        <v>86</v>
+      </c>
+      <c r="J64" t="s">
         <v>87</v>
       </c>
-      <c r="J64" t="s">
-        <v>88</v>
-      </c>
       <c r="K64" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C65" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D65" t="s">
         <v>16</v>
       </c>
       <c r="F65" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H65" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I65" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J65" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C66" t="s">
+        <v>88</v>
+      </c>
+      <c r="D66" t="s">
+        <v>25</v>
+      </c>
+      <c r="E66" t="s">
         <v>89</v>
       </c>
-      <c r="D66" t="s">
-        <v>25</v>
-      </c>
-      <c r="E66" t="s">
-        <v>90</v>
-      </c>
       <c r="H66" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I66" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C67" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D67" t="s">
         <v>16</v>
       </c>
       <c r="E67" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H67" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I67" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C68" t="s">
+        <v>91</v>
+      </c>
+      <c r="D68" t="s">
+        <v>25</v>
+      </c>
+      <c r="E68" t="s">
         <v>92</v>
       </c>
-      <c r="D68" t="s">
-        <v>25</v>
-      </c>
-      <c r="E68" t="s">
-        <v>93</v>
-      </c>
       <c r="H68" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I68" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>93</v>
+      </c>
+      <c r="C69" t="s">
+        <v>139</v>
+      </c>
+      <c r="D69" t="s">
+        <v>16</v>
+      </c>
+      <c r="F69" t="s">
         <v>94</v>
       </c>
-      <c r="C69" t="s">
-        <v>140</v>
-      </c>
-      <c r="D69" t="s">
-        <v>16</v>
-      </c>
-      <c r="F69" t="s">
-        <v>95</v>
-      </c>
       <c r="H69" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I69" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J69" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C70" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D70" t="s">
         <v>25</v>
       </c>
       <c r="F70" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H70" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I70" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J70" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B71" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C71" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D71" t="s">
         <v>16</v>
       </c>
       <c r="F71" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H71" t="s">
+        <v>96</v>
+      </c>
+      <c r="I71" t="s">
+        <v>134</v>
+      </c>
+      <c r="J71" t="s">
         <v>97</v>
       </c>
-      <c r="I71" t="s">
-        <v>135</v>
-      </c>
-      <c r="J71" t="s">
-        <v>98</v>
-      </c>
       <c r="K71" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B72" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C72" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D72" t="s">
         <v>25</v>
       </c>
       <c r="E72" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H72" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I72" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>98</v>
+      </c>
+      <c r="B73" t="s">
+        <v>163</v>
+      </c>
+      <c r="C73" t="s">
+        <v>162</v>
+      </c>
+      <c r="D73" t="s">
+        <v>16</v>
+      </c>
+      <c r="F73" t="s">
+        <v>100</v>
+      </c>
+      <c r="H73" t="s">
         <v>99</v>
       </c>
-      <c r="B73" t="s">
-        <v>164</v>
-      </c>
-      <c r="C73" t="s">
-        <v>163</v>
-      </c>
-      <c r="D73" t="s">
-        <v>16</v>
-      </c>
-      <c r="F73" t="s">
-        <v>101</v>
-      </c>
-      <c r="H73" t="s">
+      <c r="I73" t="s">
+        <v>134</v>
+      </c>
+      <c r="J73" t="s">
         <v>100</v>
       </c>
-      <c r="I73" t="s">
-        <v>135</v>
-      </c>
-      <c r="J73" t="s">
-        <v>101</v>
-      </c>
       <c r="K73" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>98</v>
+      </c>
+      <c r="B74" t="s">
+        <v>163</v>
+      </c>
+      <c r="C74" t="s">
+        <v>162</v>
+      </c>
+      <c r="D74" t="s">
+        <v>25</v>
+      </c>
+      <c r="F74" t="s">
+        <v>101</v>
+      </c>
+      <c r="H74" t="s">
         <v>99</v>
       </c>
-      <c r="B74" t="s">
-        <v>164</v>
-      </c>
-      <c r="C74" t="s">
-        <v>163</v>
-      </c>
-      <c r="D74" t="s">
-        <v>25</v>
-      </c>
-      <c r="F74" t="s">
-        <v>102</v>
-      </c>
-      <c r="H74" t="s">
-        <v>100</v>
-      </c>
       <c r="I74" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J74" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C75" t="s">
+        <v>102</v>
+      </c>
+      <c r="D75" t="s">
+        <v>16</v>
+      </c>
+      <c r="F75" t="s">
         <v>103</v>
       </c>
-      <c r="D75" t="s">
-        <v>16</v>
-      </c>
-      <c r="F75" t="s">
-        <v>104</v>
-      </c>
       <c r="H75" t="s">
+        <v>102</v>
+      </c>
+      <c r="I75" t="s">
+        <v>134</v>
+      </c>
+      <c r="J75" t="s">
         <v>103</v>
       </c>
-      <c r="I75" t="s">
-        <v>135</v>
-      </c>
-      <c r="J75" t="s">
-        <v>104</v>
-      </c>
       <c r="K75" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C76" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D76" t="s">
         <v>25</v>
       </c>
       <c r="E76" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H76" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I76" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>104</v>
+      </c>
+      <c r="C77" t="s">
         <v>105</v>
       </c>
-      <c r="C77" t="s">
+      <c r="D77" t="s">
+        <v>16</v>
+      </c>
+      <c r="E77" t="s">
         <v>106</v>
       </c>
-      <c r="D77" t="s">
-        <v>16</v>
-      </c>
-      <c r="E77" t="s">
-        <v>107</v>
-      </c>
       <c r="H77" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I77" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>104</v>
+      </c>
+      <c r="C78" t="s">
         <v>105</v>
       </c>
-      <c r="C78" t="s">
-        <v>106</v>
-      </c>
       <c r="D78" t="s">
         <v>25</v>
       </c>
       <c r="F78" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H78" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I78" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J78" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
@@ -2751,25 +2760,25 @@
         <v>22</v>
       </c>
       <c r="C79" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D79" t="s">
         <v>16</v>
       </c>
       <c r="F79" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H79" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I79" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J79" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
@@ -2777,123 +2786,123 @@
         <v>22</v>
       </c>
       <c r="C80" t="s">
+        <v>108</v>
+      </c>
+      <c r="D80" t="s">
+        <v>25</v>
+      </c>
+      <c r="E80" t="s">
         <v>109</v>
       </c>
-      <c r="D80" t="s">
-        <v>25</v>
-      </c>
-      <c r="E80" t="s">
-        <v>110</v>
-      </c>
       <c r="H80" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I80" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C81" t="s">
+        <v>111</v>
+      </c>
+      <c r="D81" t="s">
+        <v>16</v>
+      </c>
+      <c r="F81" t="s">
         <v>112</v>
       </c>
-      <c r="D81" t="s">
-        <v>16</v>
-      </c>
-      <c r="F81" t="s">
-        <v>113</v>
-      </c>
       <c r="H81" t="s">
+        <v>111</v>
+      </c>
+      <c r="I81" t="s">
+        <v>134</v>
+      </c>
+      <c r="J81" t="s">
         <v>112</v>
       </c>
-      <c r="I81" t="s">
-        <v>135</v>
-      </c>
-      <c r="J81" t="s">
-        <v>113</v>
-      </c>
       <c r="K81" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C82" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D82" t="s">
         <v>25</v>
       </c>
       <c r="F82" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H82" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I82" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J82" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C83" t="s">
+        <v>114</v>
+      </c>
+      <c r="D83" t="s">
+        <v>16</v>
+      </c>
+      <c r="F83" t="s">
         <v>115</v>
       </c>
-      <c r="D83" t="s">
-        <v>16</v>
-      </c>
-      <c r="F83" t="s">
-        <v>116</v>
-      </c>
       <c r="H83" t="s">
+        <v>114</v>
+      </c>
+      <c r="I83" t="s">
+        <v>134</v>
+      </c>
+      <c r="J83" t="s">
         <v>115</v>
       </c>
-      <c r="I83" t="s">
-        <v>135</v>
-      </c>
-      <c r="J83" t="s">
-        <v>116</v>
-      </c>
       <c r="K83" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C84" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D84" t="s">
         <v>25</v>
       </c>
       <c r="F84" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H84" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I84" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J84" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K84" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>